<commit_message>
Create Card Type Test Script
Affected files:
>Command.js
>pos-otc-data
</commit_message>
<xml_diff>
--- a/cypress/fixtures/pos-otc-data.xlsx
+++ b/cypress/fixtures/pos-otc-data.xlsx
@@ -4,21 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" activeTab="4"/>
+    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="master-itemclass-data" sheetId="1" r:id="rId1"/>
     <sheet name="itemclass-edit-el" sheetId="8" r:id="rId2"/>
-    <sheet name="itemsubclass-edit-el" sheetId="13" r:id="rId3"/>
-    <sheet name="itemclass-selector-assert" sheetId="5" r:id="rId4"/>
-    <sheet name="master-itemsubclass-data" sheetId="2" r:id="rId5"/>
-    <sheet name="master-item-data" sheetId="4" r:id="rId6"/>
-    <sheet name="master-ordertype-data" sheetId="3" r:id="rId7"/>
-    <sheet name="itemsubclass-selector-assert" sheetId="10" r:id="rId8"/>
-    <sheet name="itemclass-add-el" sheetId="6" r:id="rId9"/>
-    <sheet name="itemsubclass-add-el" sheetId="11" r:id="rId10"/>
-    <sheet name="data-to-delete" sheetId="9" r:id="rId11"/>
-    <sheet name="delete-confirm-el" sheetId="12" r:id="rId12"/>
+    <sheet name="cardtype-edit-el" sheetId="15" r:id="rId3"/>
+    <sheet name="itemsubclass-edit-el" sheetId="13" r:id="rId4"/>
+    <sheet name="itemclass-selector-assert" sheetId="5" r:id="rId5"/>
+    <sheet name="module-selector-assert" sheetId="16" r:id="rId6"/>
+    <sheet name="master-itemsubclass-data" sheetId="2" r:id="rId7"/>
+    <sheet name="master-item-data" sheetId="4" r:id="rId8"/>
+    <sheet name="master-ordertype-data" sheetId="3" r:id="rId9"/>
+    <sheet name="itemsubclass-selector-assert" sheetId="10" r:id="rId10"/>
+    <sheet name="itemclass-add-el" sheetId="6" r:id="rId11"/>
+    <sheet name="cardtype-add-el" sheetId="17" r:id="rId12"/>
+    <sheet name="itemsubclass-add-el" sheetId="11" r:id="rId13"/>
+    <sheet name="data-to-delete" sheetId="9" r:id="rId14"/>
+    <sheet name="delete-confirm-el" sheetId="12" r:id="rId15"/>
+    <sheet name="master-cardtype-data" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="129">
   <si>
     <t>itemClass</t>
   </si>
@@ -133,6 +137,12 @@
     <t>Save button should contain text "Save" instead of "Update Data"</t>
   </si>
   <si>
+    <t>Cancel button should contain text "Cancel" instead of "update Data"</t>
+  </si>
+  <si>
+    <t>#cardtype</t>
+  </si>
+  <si>
     <t>#itemsubclassdsc</t>
   </si>
   <si>
@@ -364,6 +374,12 @@
     <t>"Save" button Should be enabled and clickable</t>
   </si>
   <si>
+    <t>Save button should contain text "Save" instead of "Add Data"</t>
+  </si>
+  <si>
+    <t>Cancel button should contain text "Cancel"</t>
+  </si>
+  <si>
     <t>Save button should contain text "Save"</t>
   </si>
   <si>
@@ -383,6 +399,36 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>cardType</t>
+  </si>
+  <si>
+    <t>editCardType</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Debit Card</t>
+  </si>
+  <si>
+    <t>Prepaid Card</t>
+  </si>
+  <si>
+    <t>Gift Card</t>
+  </si>
+  <si>
+    <t>Store Gift</t>
+  </si>
+  <si>
+    <t>Store Card</t>
+  </si>
+  <si>
+    <t>Loyalty Card</t>
+  </si>
+  <si>
+    <t>Electronic Card</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1370,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1402,6 +1448,375 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="17.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="32.5714285714286" customWidth="1"/>
+    <col min="4" max="5" width="14.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="32.5714285714286" customWidth="1"/>
+    <col min="4" max="5" width="14.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E7"/>
@@ -1441,7 +1856,7 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1455,29 +1870,29 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1488,7 +1903,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1508,7 +1923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:A4"/>
@@ -1521,7 +1936,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1545,13 +1960,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1575,30 +1990,116 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1613,7 +2114,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
@@ -1704,6 +2205,102 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="32.5714285714286" customWidth="1"/>
+    <col min="4" max="5" width="14.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E7"/>
@@ -1762,24 +2359,24 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1790,7 +2387,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1810,7 +2407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D11"/>
@@ -1829,7 +2426,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -1843,142 +2440,142 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1987,13 +2584,190 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="17.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -2004,13 +2778,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2018,13 +2792,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -2032,7 +2806,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -2040,7 +2814,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2048,7 +2822,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -2056,7 +2830,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -2064,7 +2838,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -2072,7 +2846,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -2080,7 +2854,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -2088,7 +2862,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -2096,7 +2870,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -2104,7 +2878,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -2112,7 +2886,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -2120,7 +2894,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2128,7 +2902,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2172,7 +2946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:A13"/>
@@ -2188,289 +2962,67 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="17.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2482,91 +3034,40 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
-  <cols>
-    <col min="1" max="1" width="32.5714285714286" customWidth="1"/>
-    <col min="4" max="5" width="14.8571428571429" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate report free reasons
</commit_message>
<xml_diff>
--- a/cypress/fixtures/pos-otc-data.xlsx
+++ b/cypress/fixtures/pos-otc-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="30" activeTab="35"/>
+    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="29" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="master-itemclass-data" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="333">
   <si>
     <t>itemClass</t>
   </si>
@@ -685,49 +685,55 @@
     <t>This is a very long string that exceeds the maximum allowed length.</t>
   </si>
   <si>
+    <t>freeReasons</t>
+  </si>
+  <si>
+    <t>editFreeReasons</t>
+  </si>
+  <si>
+    <t>onlySearch</t>
+  </si>
+  <si>
+    <t>onlyDelete</t>
+  </si>
+  <si>
+    <t>Sample Giveaway</t>
+  </si>
+  <si>
+    <t>Customer Complaint Resolution</t>
+  </si>
+  <si>
+    <t>Complimentary Item</t>
+  </si>
+  <si>
+    <t>Birthday Freebie</t>
+  </si>
+  <si>
+    <t>Employee Perk</t>
+  </si>
+  <si>
+    <t>Sampling</t>
+  </si>
+  <si>
+    <t>Coupon Redemption</t>
+  </si>
+  <si>
+    <t>Membership Perk</t>
+  </si>
+  <si>
+    <t>Incorrect Charge</t>
+  </si>
+  <si>
+    <t>Inventory Clearance</t>
+  </si>
+  <si>
+    <t>Customer Appreciation</t>
+  </si>
+  <si>
     <t>voidReasons</t>
   </si>
   <si>
     <t>editVoidReasons</t>
-  </si>
-  <si>
-    <t>onlySearch</t>
-  </si>
-  <si>
-    <t>onlyDelete</t>
-  </si>
-  <si>
-    <t>Sample Giveaway</t>
-  </si>
-  <si>
-    <t>Customer Complaint Resolution</t>
-  </si>
-  <si>
-    <t>Complimentary Item</t>
-  </si>
-  <si>
-    <t>Birthday Freebie</t>
-  </si>
-  <si>
-    <t>Employee Perk</t>
-  </si>
-  <si>
-    <t>Sampling</t>
-  </si>
-  <si>
-    <t>Coupon Redemption</t>
-  </si>
-  <si>
-    <t>Membership Perk</t>
-  </si>
-  <si>
-    <t>Incorrect Charge</t>
-  </si>
-  <si>
-    <t>Inventory Clearance</t>
-  </si>
-  <si>
-    <t>Customer Appreciation</t>
   </si>
   <si>
     <t>Incorrect Order Entry</t>
@@ -1067,13 +1073,19 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -1538,16 +1550,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1556,125 +1565,132 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2586,7 +2602,7 @@
       <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2658,7 +2674,7 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D19" t="s">
@@ -2672,7 +2688,7 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="6" t="s">
         <v>114</v>
       </c>
       <c r="D20" t="s">
@@ -2686,7 +2702,7 @@
       <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D21" t="s">
@@ -2820,7 +2836,7 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B31" t="s">
@@ -4810,13 +4826,13 @@
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="54.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="39.1428571428571" customWidth="1"/>
@@ -4838,7 +4854,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -4848,8 +4864,9 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -4859,8 +4876,9 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -4870,8 +4888,9 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -4881,8 +4900,9 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>215</v>
       </c>
@@ -4892,8 +4912,9 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -4903,8 +4924,9 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>217</v>
       </c>
@@ -4914,8 +4936,9 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>218</v>
       </c>
@@ -4928,6 +4951,7 @@
       <c r="D9" t="b">
         <v>0</v>
       </c>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -5020,10 +5044,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="C1" t="s">
         <v>209</v>
@@ -5034,7 +5058,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -5045,7 +5069,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -5056,7 +5080,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -5067,7 +5091,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -5078,7 +5102,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -5089,7 +5113,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -5100,7 +5124,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -5111,7 +5135,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
         <v>219</v>
@@ -5125,7 +5149,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -5136,7 +5160,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -5216,30 +5240,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s">
         <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D1" t="s">
         <v>154</v>
       </c>
       <c r="E1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F1" t="s">
         <v>210</v>
       </c>
       <c r="G1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
         <v>159</v>
@@ -5256,10 +5280,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -5273,10 +5297,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -5290,10 +5314,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" t="s">
         <v>240</v>
-      </c>
-      <c r="B5" t="s">
-        <v>238</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -5307,7 +5331,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
         <v>162</v>
@@ -5324,7 +5348,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
         <v>165</v>
@@ -5341,7 +5365,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
         <v>165</v>
@@ -5358,13 +5382,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B9" t="s">
         <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
         <v>165</v>
@@ -5381,7 +5405,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B10" t="s">
         <v>160</v>
@@ -5398,7 +5422,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>162</v>
@@ -5543,22 +5567,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G1" t="s">
         <v>210</v>
@@ -5566,10 +5590,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -5583,10 +5607,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -5600,16 +5624,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
         <v>257</v>
-      </c>
-      <c r="D4" t="s">
-        <v>255</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -5623,10 +5647,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -5640,10 +5664,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -5660,7 +5684,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -5677,7 +5701,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -5694,7 +5718,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -5711,7 +5735,7 @@
         <v>206</v>
       </c>
       <c r="B10" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -5781,55 +5805,55 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="J1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="K1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="L1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="M1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="N1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="O1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="P1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="Q1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:17">
@@ -5837,46 +5861,46 @@
         <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="I2" s="1">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="K2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="N2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="P2" t="b">
         <v>1</v>
@@ -5890,46 +5914,46 @@
         <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H3" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="K3" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="N3" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O3" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>
@@ -5943,46 +5967,46 @@
         <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F4" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H4" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="K4" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="L4" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="N4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="O4" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="P4" t="b">
         <v>0</v>
@@ -6055,15 +6079,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -6077,7 +6101,7 @@
   <sheetPr/>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -6085,87 +6109,87 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="G1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="I1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="J1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="K1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="L1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="M1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="N1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="O1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F2" t="s">
         <v>190</v>
       </c>
       <c r="G2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="I2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="J2" t="s">
-        <v>325</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>328</v>
       </c>
       <c r="L2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
@@ -6176,40 +6200,40 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E3" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F3" t="s">
         <v>190</v>
       </c>
       <c r="G3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="H3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="I3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J3" t="s">
-        <v>328</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="L3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
update and generate report
</commit_message>
<xml_diff>
--- a/cypress/fixtures/pos-otc-data.xlsx
+++ b/cypress/fixtures/pos-otc-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="32" activeTab="38"/>
+    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="16" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="master-itemclass-data" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="403">
   <si>
     <t>itemClass</t>
   </si>
@@ -106,12 +106,12 @@
     <t>null</t>
   </si>
   <si>
+    <t>© ™ ® à á â ñ ä ¢ £ ¥ € ! @ # $ ^ * _ + = &lt; &gt; ? ` \ ~ \" | \ ] [ ] ; :</t>
+  </si>
+  <si>
     <t>Jollibee Filipino Sweet Style Spaghetti Langhap Sarap</t>
   </si>
   <si>
-    <t>©™®àáâñä¢£¥€!@#$^*_+=&lt;&gt;?`~"|\ [];:</t>
-  </si>
-  <si>
     <t>sel</t>
   </si>
   <si>
@@ -580,9 +580,6 @@
     <t>Juices</t>
   </si>
   <si>
-    <t>© ™ ® à á â ñ ä ¢ £ ¥ € ! @ # $ ^ * _ + = &lt; &gt; ? ` \ ~ \" | \ ] [ ] ; :</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -682,13 +679,16 @@
     <t>00000000007</t>
   </si>
   <si>
+    <t>00000000008</t>
+  </si>
+  <si>
+    <t>00000000010</t>
+  </si>
+  <si>
+    <t>© ™ ® à á â ñ ä ¢ £ ¥ € ! @ # $ ^ * _ + = &lt; &gt; ? ` \\ ~ \\\" | \\ ] [ ] ; :</t>
+  </si>
+  <si>
     <t>!@#$%^&amp;*()</t>
-  </si>
-  <si>
-    <t>00000000009</t>
-  </si>
-  <si>
-    <t>00000000010</t>
   </si>
   <si>
     <t>This is a very long string that exceeds the maximum allowed length.</t>
@@ -2229,8 +2229,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3733,7 +3733,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -3741,7 +3741,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -3758,8 +3758,8 @@
   <sheetPr/>
   <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3769,10 +3769,10 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
         <v>172</v>
-      </c>
-      <c r="B1" t="s">
-        <v>173</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -3781,34 +3781,34 @@
         <v>156</v>
       </c>
       <c r="E1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>175</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>176</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>177</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>178</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>179</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>180</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>181</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>182</v>
-      </c>
-      <c r="N1" t="s">
-        <v>183</v>
       </c>
       <c r="O1" t="s">
         <v>2</v>
@@ -3820,10 +3820,10 @@
         <v>4</v>
       </c>
       <c r="R1" t="s">
+        <v>183</v>
+      </c>
+      <c r="S1" t="s">
         <v>184</v>
-      </c>
-      <c r="S1" t="s">
-        <v>185</v>
       </c>
       <c r="T1" t="s">
         <v>1</v>
@@ -3832,42 +3832,42 @@
         <v>156</v>
       </c>
       <c r="V1" t="s">
+        <v>173</v>
+      </c>
+      <c r="W1" t="s">
         <v>174</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>175</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>176</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>177</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>178</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>179</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>180</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>181</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>182</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
         <v>186</v>
-      </c>
-      <c r="B2" t="s">
-        <v>187</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3876,13 +3876,13 @@
         <v>163</v>
       </c>
       <c r="E2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="H2">
         <v>40</v>
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
@@ -3905,10 +3905,10 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -3917,13 +3917,13 @@
         <v>162</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H3">
         <v>76</v>
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
@@ -3946,10 +3946,10 @@
     </row>
     <row r="4" spans="1:27">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -3958,13 +3958,13 @@
         <v>167</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H4">
         <v>63</v>
@@ -3973,7 +3973,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
@@ -3985,10 +3985,10 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T4" t="s">
         <v>7</v>
@@ -3997,13 +3997,13 @@
         <v>169</v>
       </c>
       <c r="V4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Y4">
         <v>80</v>
@@ -4012,15 +4012,15 @@
         <v>1</v>
       </c>
       <c r="AA4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -4029,13 +4029,13 @@
         <v>169</v>
       </c>
       <c r="E5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H5">
         <v>48</v>
@@ -4044,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -4058,10 +4058,10 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -4070,13 +4070,13 @@
         <v>162</v>
       </c>
       <c r="E6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6">
         <v>449</v>
@@ -4085,7 +4085,7 @@
         <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O6" t="b">
         <v>0</v>
@@ -4099,25 +4099,25 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="E7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>202</v>
       </c>
       <c r="H7">
         <v>50</v>
@@ -4126,7 +4126,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O7" t="b">
         <v>0</v>
@@ -4140,10 +4140,10 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -4152,13 +4152,13 @@
         <v>162</v>
       </c>
       <c r="E8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H8">
         <v>50</v>
@@ -4167,13 +4167,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O8" t="b">
         <v>0</v>
       </c>
       <c r="P8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="b">
         <v>0</v>
@@ -4184,7 +4184,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -4193,13 +4193,13 @@
         <v>162</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" t="s">
-        <v>205</v>
+      <c r="G9" s="7" t="s">
+        <v>204</v>
       </c>
       <c r="H9">
         <v>51</v>
@@ -4208,7 +4208,7 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O9" t="b">
         <v>0</v>
@@ -4222,10 +4222,10 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -4234,28 +4234,28 @@
         <v>162</v>
       </c>
       <c r="E10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H10">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O10" t="b">
         <v>0</v>
       </c>
       <c r="P10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="b">
         <v>0</v>
@@ -4263,10 +4263,10 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -4275,22 +4275,22 @@
         <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" t="s">
         <v>207</v>
       </c>
       <c r="H11">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O11" t="b">
         <v>0</v>
@@ -4307,7 +4307,7 @@
         <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -4316,7 +4316,7 @@
         <v>162</v>
       </c>
       <c r="E12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -4331,7 +4331,7 @@
         <v>5</v>
       </c>
       <c r="J12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O12" t="b">
         <v>0</v>
@@ -5427,13 +5427,13 @@
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -5447,7 +5447,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5590,12 +5595,12 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5787,7 +5792,7 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -5977,7 +5982,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -6009,7 +6014,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6171,7 +6176,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -6188,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6203,7 +6208,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -6451,7 +6456,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>165</v>
@@ -6460,7 +6465,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -6693,7 +6698,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>283</v>
@@ -7470,8 +7475,8 @@
   <sheetPr/>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
Run 2 Card Type
</commit_message>
<xml_diff>
--- a/cypress/fixtures/pos-otc-data.xlsx
+++ b/cypress/fixtures/pos-otc-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="33" activeTab="39"/>
+    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="28" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="master-itemclass-data" sheetId="1" r:id="rId1"/>
@@ -6796,8 +6796,8 @@
   <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6896,7 +6896,7 @@
         <v>13</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -8387,7 +8387,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="I4 F2:F3" numberStoredAsText="1"/>
+    <ignoredError sqref="F2:F3 I4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9148,7 +9148,7 @@
   <sheetPr/>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -9989,7 +9989,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A15:A16 B15:B16" numberStoredAsText="1"/>
+    <ignoredError sqref="B15:B16 A15:A16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Run 2 Payment Type
</commit_message>
<xml_diff>
--- a/cypress/fixtures/pos-otc-data.xlsx
+++ b/cypress/fixtures/pos-otc-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500" tabRatio="942" firstSheet="28" activeTab="28"/>
+    <workbookView windowWidth="19635" windowHeight="7050" tabRatio="942" firstSheet="29" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="master-itemclass-data" sheetId="1" r:id="rId1"/>
@@ -6796,7 +6796,7 @@
   <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -7014,8 +7014,8 @@
   <sheetPr/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7138,7 +7138,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -8387,7 +8387,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="F2:F3 I4" numberStoredAsText="1"/>
+    <ignoredError sqref="I4 F2:F3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9989,7 +9989,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="B15:B16 A15:A16" numberStoredAsText="1"/>
+    <ignoredError sqref="A15:A16 B15:B16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Run 2 Void Refund Reasons
</commit_message>
<xml_diff>
--- a/cypress/fixtures/pos-otc-data.xlsx
+++ b/cypress/fixtures/pos-otc-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7050" tabRatio="942" firstSheet="29" activeTab="29"/>
+    <workbookView windowWidth="19635" windowHeight="7050" tabRatio="942" firstSheet="29" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="master-itemclass-data" sheetId="1" r:id="rId1"/>
@@ -7014,7 +7014,7 @@
   <sheetPr/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -7362,8 +7362,8 @@
   <sheetPr/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7531,7 +7531,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -8387,7 +8387,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="I4 F2:F3" numberStoredAsText="1"/>
+    <ignoredError sqref="F2:F3 I4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9989,7 +9989,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A15:A16 B15:B16" numberStoredAsText="1"/>
+    <ignoredError sqref="B15:B16 A15:A16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>